<commit_message>
commit by Kristina in 20241019
</commit_message>
<xml_diff>
--- a/table4.xlsx
+++ b/table4.xlsx
@@ -77,88 +77,88 @@
     <t xml:space="preserve">Rho_m(Rf)</t>
   </si>
   <si>
-    <t xml:space="preserve">1935-01-01 to 2022-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1935-01-01 to 1945-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1946-01-01 to 1955-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1956-01-01 to 1965-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1966-01-01 to 1975-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1976-01-01 to 1985-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1986-01-01 to 1995-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1996-01-01 to 2005-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2006-01-01 to 2015-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-01-01 to 2022-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1935-01-01 to 1940-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1941-01-01 to 1945-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1946-01-01 to 1950-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1951-01-01 to 1955-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1956-01-01 to 1960-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1961-01-01 to 1965-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1966-01-01 to 1970-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1971-01-01 to 1975-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1976-01-01 to 1980-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1981-01-01 to 1985-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1986-01-01 to 1990-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1991-01-01 to 1995-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1996-01-01 to 2000-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2001-01-01 to 2005-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2006-01-01 to 2010-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011-01-01 to 2015-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-01-01 to 2020-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021-01-01 to 2022-12-31</t>
+    <t xml:space="preserve">1935-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1935-1945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1946-1955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1956-1965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1966-1975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1976-1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1986-1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1996-2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2006-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1935-1940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1941-1945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1946-1950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1951-1955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1956-1960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1961-1965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1966-1970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1971-1975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1976-1980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1981-1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1986-1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1991-1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1996-2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2006-2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-2022</t>
   </si>
 </sst>
 </file>
@@ -560,64 +560,64 @@
         <v>21</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0125128519953952</v>
+        <v>0.013</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.262686011640969</v>
+        <v>-0.263</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00760660758961107</v>
+        <v>0.008</v>
       </c>
       <c r="E2" t="n">
-        <v>0.00494323173305047</v>
+        <v>0.005</v>
       </c>
       <c r="F2" t="n">
-        <v>0.275198863636364</v>
+        <v>0.275</v>
       </c>
       <c r="G2" t="n">
-        <v>-4.64770502337665</v>
+        <v>-4.648</v>
       </c>
       <c r="H2" t="n">
-        <v>0.134583749184978</v>
+        <v>0.135</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0565195102356392</v>
+        <v>0.057</v>
       </c>
       <c r="J2" t="n">
-        <v>0.265847554000764</v>
+        <v>0.266</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0125521974982263</v>
+        <v>0.013</v>
       </c>
       <c r="L2" t="n">
-        <v>0.258191960327687</v>
+        <v>0.258</v>
       </c>
       <c r="M2" t="n">
-        <v>7.19432208370528</v>
+        <v>7.194</v>
       </c>
       <c r="N2" t="n">
-        <v>-32.1096991838525</v>
+        <v>-32.11</v>
       </c>
       <c r="O2" t="n">
-        <v>2.43099572605449</v>
+        <v>2.431</v>
       </c>
       <c r="P2" t="n">
-        <v>2.75235921457805</v>
+        <v>2.752</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0819998669786308</v>
+        <v>0.082</v>
       </c>
       <c r="R2" t="n">
-        <v>0.936966214221095</v>
+        <v>0.937</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0584896595320377</v>
+        <v>0.058</v>
       </c>
       <c r="T2" t="n">
-        <v>0.057219348935585</v>
+        <v>0.057</v>
       </c>
       <c r="U2" t="n">
-        <v>0.979260430869433</v>
+        <v>0.979</v>
       </c>
     </row>
     <row r="3">
@@ -625,64 +625,64 @@
         <v>22</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0197017486568473</v>
+        <v>0.02</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00538356683866552</v>
+        <v>0.005</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0231863204171875</v>
+        <v>0.023</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.0042176517967461</v>
+        <v>-0.004</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0143181818181818</v>
+        <v>0.014</v>
       </c>
       <c r="G3" t="n">
-        <v>0.060765008615292</v>
+        <v>0.061</v>
       </c>
       <c r="H3" t="n">
-        <v>0.261706969028096</v>
+        <v>0.262</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0885964959331989</v>
+        <v>0.089</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0872661416312728</v>
+        <v>0.087</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0219547299037708</v>
+        <v>0.022</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0154915974180234</v>
+        <v>0.015</v>
       </c>
       <c r="M3" t="n">
-        <v>2.55490757763019</v>
+        <v>2.555</v>
       </c>
       <c r="N3" t="n">
-        <v>0.708779748673018</v>
+        <v>0.709</v>
       </c>
       <c r="O3" t="n">
-        <v>1.66359048386966</v>
+        <v>1.664</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.497594714767263</v>
+        <v>-0.498</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.063010658850094</v>
+        <v>-0.063</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.0295871191115476</v>
+        <v>-0.03</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.0788277852576836</v>
+        <v>-0.079</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.0456679764326316</v>
+        <v>-0.046</v>
       </c>
       <c r="U3" t="n">
-        <v>0.635897938118192</v>
+        <v>0.636</v>
       </c>
     </row>
     <row r="4">
@@ -690,64 +690,64 @@
         <v>23</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0112318361740467</v>
+        <v>0.011</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0832681638259533</v>
+        <v>-0.083</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00204641381056375</v>
+        <v>0.002</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00925502280882393</v>
+        <v>0.009</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0945</v>
+        <v>0.094</v>
       </c>
       <c r="G4" t="n">
-        <v>-1.92027175965643</v>
+        <v>-1.92</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0471929542869501</v>
+        <v>0.047</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0433626977052724</v>
+        <v>0.043</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0603023006391169</v>
+        <v>0.06</v>
       </c>
       <c r="K4" t="n">
-        <v>0.00921077401381653</v>
+        <v>0.009</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0438839186870057</v>
+        <v>0.044</v>
       </c>
       <c r="M4" t="n">
-        <v>2.83742956978431</v>
+        <v>2.837</v>
       </c>
       <c r="N4" t="n">
-        <v>-15.1264051839261</v>
+        <v>-15.126</v>
       </c>
       <c r="O4" t="n">
-        <v>0.357246957091226</v>
+        <v>0.357</v>
       </c>
       <c r="P4" t="n">
-        <v>3.07337750834553</v>
+        <v>3.073</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0872247435417927</v>
+        <v>0.087</v>
       </c>
       <c r="R4" t="n">
-        <v>0.455760662629811</v>
+        <v>0.456</v>
       </c>
       <c r="S4" t="n">
-        <v>0.000609508457083087</v>
+        <v>0.001</v>
       </c>
       <c r="T4" t="n">
-        <v>0.00247844056819828</v>
+        <v>0.002</v>
       </c>
       <c r="U4" t="n">
-        <v>0.892337190994264</v>
+        <v>0.892</v>
       </c>
     </row>
     <row r="5">
@@ -755,64 +755,64 @@
         <v>24</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0111759118948601</v>
+        <v>0.011</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.220740754771807</v>
+        <v>-0.221</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0065321666230439</v>
+        <v>0.007</v>
       </c>
       <c r="E5" t="n">
-        <v>0.00494017354852007</v>
+        <v>0.005</v>
       </c>
       <c r="F5" t="n">
-        <v>0.231916666666667</v>
+        <v>0.232</v>
       </c>
       <c r="G5" t="n">
-        <v>-5.8556192102127</v>
+        <v>-5.856</v>
       </c>
       <c r="H5" t="n">
-        <v>0.173279648344717</v>
+        <v>0.173</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0376972523054122</v>
+        <v>0.038</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0805818498338415</v>
+        <v>0.081</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0109238409724884</v>
+        <v>0.011</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0667655604037172</v>
+        <v>0.067</v>
       </c>
       <c r="M5" t="n">
-        <v>3.24761019498833</v>
+        <v>3.248</v>
       </c>
       <c r="N5" t="n">
-        <v>-30.0079213864011</v>
+        <v>-30.008</v>
       </c>
       <c r="O5" t="n">
-        <v>1.02128451758017</v>
+        <v>1.021</v>
       </c>
       <c r="P5" t="n">
-        <v>1.36181705701005</v>
+        <v>1.362</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.121519823818755</v>
+        <v>0.122</v>
       </c>
       <c r="R5" t="n">
-        <v>0.667071576333786</v>
+        <v>0.667</v>
       </c>
       <c r="S5" t="n">
-        <v>0.0463676748430232</v>
+        <v>0.046</v>
       </c>
       <c r="T5" t="n">
-        <v>0.0941355583527158</v>
+        <v>0.094</v>
       </c>
       <c r="U5" t="n">
-        <v>0.751524943585634</v>
+        <v>0.752</v>
       </c>
     </row>
     <row r="6">
@@ -820,64 +820,64 @@
         <v>25</v>
       </c>
       <c r="B6" t="n">
-        <v>0.00663794764896117</v>
+        <v>0.007</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.449612052351039</v>
+        <v>-0.45</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0055294033146334</v>
+        <v>0.006</v>
       </c>
       <c r="E6" t="n">
-        <v>0.000837438627800473</v>
+        <v>0.001</v>
       </c>
       <c r="F6" t="n">
-        <v>0.45625</v>
+        <v>0.456</v>
       </c>
       <c r="G6" t="n">
-        <v>-6.8552158802801</v>
+        <v>-6.855</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0843065776656569</v>
+        <v>0.084</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0655868553526382</v>
+        <v>0.066</v>
       </c>
       <c r="J6" t="n">
-        <v>0.146349756945091</v>
+        <v>0.146</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0123954992927038</v>
+        <v>0.012</v>
       </c>
       <c r="L6" t="n">
-        <v>0.118902986371526</v>
+        <v>0.119</v>
       </c>
       <c r="M6" t="n">
-        <v>1.10868363586765</v>
+        <v>1.109</v>
       </c>
       <c r="N6" t="n">
-        <v>-33.6539900495021</v>
+        <v>-33.654</v>
       </c>
       <c r="O6" t="n">
-        <v>0.532337473591919</v>
+        <v>0.532</v>
       </c>
       <c r="P6" t="n">
-        <v>0.148142265168947</v>
+        <v>0.148</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.171304824491052</v>
+        <v>0.171</v>
       </c>
       <c r="R6" t="n">
-        <v>0.708731113112997</v>
+        <v>0.709</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0274505636766493</v>
+        <v>0.027</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.0598623840462043</v>
+        <v>-0.06</v>
       </c>
       <c r="U6" t="n">
-        <v>0.835602196047388</v>
+        <v>0.836</v>
       </c>
     </row>
     <row r="7">
@@ -885,64 +885,64 @@
         <v>26</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0207429511140181</v>
+        <v>0.021</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.702590382219315</v>
+        <v>-0.703</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0129660709580516</v>
+        <v>0.013</v>
       </c>
       <c r="E7" t="n">
-        <v>0.00655172333630227</v>
+        <v>0.007</v>
       </c>
       <c r="F7" t="n">
-        <v>0.723333333333333</v>
+        <v>0.723</v>
       </c>
       <c r="G7" t="n">
-        <v>-13.4099172111072</v>
+        <v>-13.41</v>
       </c>
       <c r="H7" t="n">
-        <v>0.247475545497202</v>
+        <v>0.247</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0523933422674208</v>
+        <v>0.052</v>
       </c>
       <c r="J7" t="n">
-        <v>0.26162936080557</v>
+        <v>0.262</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0116258228661108</v>
+        <v>0.012</v>
       </c>
       <c r="L7" t="n">
-        <v>0.246870609913808</v>
+        <v>0.247</v>
       </c>
       <c r="M7" t="n">
-        <v>4.33695646915787</v>
+        <v>4.337</v>
       </c>
       <c r="N7" t="n">
-        <v>-29.4175393650622</v>
+        <v>-29.418</v>
       </c>
       <c r="O7" t="n">
-        <v>1.49102804886522</v>
+        <v>1.491</v>
       </c>
       <c r="P7" t="n">
-        <v>1.3592708146571</v>
+        <v>1.359</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.120187989103583</v>
+        <v>0.12</v>
       </c>
       <c r="R7" t="n">
-        <v>0.880703306462279</v>
+        <v>0.881</v>
       </c>
       <c r="S7" t="n">
-        <v>0.142464781103435</v>
+        <v>0.142</v>
       </c>
       <c r="T7" t="n">
-        <v>0.214873473158597</v>
+        <v>0.215</v>
       </c>
       <c r="U7" t="n">
-        <v>0.909107321966763</v>
+        <v>0.909</v>
       </c>
     </row>
     <row r="8">
@@ -950,64 +950,64 @@
         <v>27</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0125847886674351</v>
+        <v>0.013</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.439165211332565</v>
+        <v>-0.439</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00690568418129436</v>
+        <v>0.007</v>
       </c>
       <c r="E8" t="n">
-        <v>0.00564649301598099</v>
+        <v>0.006</v>
       </c>
       <c r="F8" t="n">
-        <v>0.45175</v>
+        <v>0.452</v>
       </c>
       <c r="G8" t="n">
-        <v>-9.53583533798709</v>
+        <v>-9.536</v>
       </c>
       <c r="H8" t="n">
-        <v>0.149946911890291</v>
+        <v>0.15</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0460541940760135</v>
+        <v>0.046</v>
       </c>
       <c r="J8" t="n">
-        <v>0.156812405715271</v>
+        <v>0.157</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0138633952450886</v>
+        <v>0.014</v>
       </c>
       <c r="L8" t="n">
-        <v>0.144534387173538</v>
+        <v>0.145</v>
       </c>
       <c r="M8" t="n">
-        <v>2.99341798195949</v>
+        <v>2.993</v>
       </c>
       <c r="N8" t="n">
-        <v>-30.6787835593986</v>
+        <v>-30.679</v>
       </c>
       <c r="O8" t="n">
-        <v>0.8433759761617</v>
+        <v>0.843</v>
       </c>
       <c r="P8" t="n">
-        <v>1.14546952350602</v>
+        <v>1.145</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.222474135098088</v>
+        <v>0.222</v>
       </c>
       <c r="R8" t="n">
-        <v>0.823534379911158</v>
+        <v>0.824</v>
       </c>
       <c r="S8" t="n">
-        <v>0.279730373659683</v>
+        <v>0.28</v>
       </c>
       <c r="T8" t="n">
-        <v>0.272615250931318</v>
+        <v>0.273</v>
       </c>
       <c r="U8" t="n">
-        <v>0.919926782384665</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="9">
@@ -1015,64 +1015,64 @@
         <v>28</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0125331735912413</v>
+        <v>0.013</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.285800159742092</v>
+        <v>-0.286</v>
       </c>
       <c r="D9" t="n">
-        <v>0.00447438951535537</v>
+        <v>0.004</v>
       </c>
       <c r="E9" t="n">
-        <v>0.00873135718453213</v>
+        <v>0.009</v>
       </c>
       <c r="F9" t="n">
-        <v>0.298333333333333</v>
+        <v>0.298</v>
       </c>
       <c r="G9" t="n">
-        <v>-6.87576200386855</v>
+        <v>-6.876</v>
       </c>
       <c r="H9" t="n">
-        <v>0.10764457741364</v>
+        <v>0.108</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0415663252423936</v>
+        <v>0.042</v>
       </c>
       <c r="J9" t="n">
-        <v>0.155920216332413</v>
+        <v>0.156</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0126842865006171</v>
+        <v>0.013</v>
       </c>
       <c r="L9" t="n">
-        <v>0.148104739983575</v>
+        <v>0.148</v>
       </c>
       <c r="M9" t="n">
-        <v>3.30301120102363</v>
+        <v>3.303</v>
       </c>
       <c r="N9" t="n">
-        <v>-20.0793967724609</v>
+        <v>-20.079</v>
       </c>
       <c r="O9" t="n">
-        <v>0.499738631510982</v>
+        <v>0.5</v>
       </c>
       <c r="P9" t="n">
-        <v>1.56169242802498</v>
+        <v>1.562</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.183291065308673</v>
+        <v>0.183</v>
       </c>
       <c r="R9" t="n">
-        <v>0.915009026276905</v>
+        <v>0.915</v>
       </c>
       <c r="S9" t="n">
-        <v>0.11106421085841</v>
+        <v>0.111</v>
       </c>
       <c r="T9" t="n">
-        <v>0.088435914871417</v>
+        <v>0.088</v>
       </c>
       <c r="U9" t="n">
-        <v>0.961908966986967</v>
+        <v>0.962</v>
       </c>
     </row>
     <row r="10">
@@ -1080,64 +1080,64 @@
         <v>29</v>
       </c>
       <c r="B10" t="n">
-        <v>0.00760100059260187</v>
+        <v>0.008</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0853989994073981</v>
+        <v>-0.085</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.00120535195183584</v>
+        <v>-0.001</v>
       </c>
       <c r="E10" t="n">
-        <v>0.00934931407701512</v>
+        <v>0.009</v>
       </c>
       <c r="F10" t="n">
         <v>0.093</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.57673220483334</v>
+        <v>-1.577</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.0222545609879083</v>
+        <v>-0.022</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0541620188549549</v>
+        <v>0.054</v>
       </c>
       <c r="J10" t="n">
-        <v>0.166047019931005</v>
+        <v>0.166</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0102509111098904</v>
+        <v>0.01</v>
       </c>
       <c r="L10" t="n">
-        <v>0.154781494127592</v>
+        <v>0.155</v>
       </c>
       <c r="M10" t="n">
-        <v>1.53732802882672</v>
+        <v>1.537</v>
       </c>
       <c r="N10" t="n">
-        <v>-5.63394132375733</v>
+        <v>-5.634</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.134821628572457</v>
+        <v>-0.135</v>
       </c>
       <c r="P10" t="n">
-        <v>2.0785470221761</v>
+        <v>2.079</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.212966347835144</v>
+        <v>0.213</v>
       </c>
       <c r="R10" t="n">
-        <v>0.904175925933348</v>
+        <v>0.904</v>
       </c>
       <c r="S10" t="n">
-        <v>0.237971971684153</v>
+        <v>0.238</v>
       </c>
       <c r="T10" t="n">
-        <v>0.17629769747242</v>
+        <v>0.176</v>
       </c>
       <c r="U10" t="n">
-        <v>0.990385100445448</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="11">
@@ -1145,64 +1145,64 @@
         <v>30</v>
       </c>
       <c r="B11" t="n">
-        <v>0.00847652050540217</v>
+        <v>0.008</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0728330033041217</v>
+        <v>-0.073</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0059777398265209</v>
+        <v>0.006</v>
       </c>
       <c r="E11" t="n">
-        <v>0.00404047661184266</v>
+        <v>0.004</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0813095238095238</v>
+        <v>0.081</v>
       </c>
       <c r="G11" t="n">
-        <v>-1.25486002484536</v>
+        <v>-1.255</v>
       </c>
       <c r="H11" t="n">
-        <v>0.102992138274251</v>
+        <v>0.103</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0580407390960575</v>
+        <v>0.058</v>
       </c>
       <c r="J11" t="n">
-        <v>0.109155052855732</v>
+        <v>0.109</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0076494358421823</v>
+        <v>0.008</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0814888529874871</v>
+        <v>0.081</v>
       </c>
       <c r="M11" t="n">
-        <v>1.33851833904332</v>
+        <v>1.339</v>
       </c>
       <c r="N11" t="n">
-        <v>-6.11538800999407</v>
+        <v>-6.115</v>
       </c>
       <c r="O11" t="n">
-        <v>0.654783708256515</v>
+        <v>0.655</v>
       </c>
       <c r="P11" t="n">
-        <v>0.890127105891911</v>
+        <v>0.89</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.0631890158870519</v>
+        <v>-0.063</v>
       </c>
       <c r="R11" t="n">
-        <v>0.598461281599629</v>
+        <v>0.598</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.0968454669371668</v>
+        <v>-0.097</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.114434697399302</v>
+        <v>-0.114</v>
       </c>
       <c r="U11" t="n">
-        <v>0.953174033304445</v>
+        <v>0.953</v>
       </c>
     </row>
     <row r="12">
@@ -1210,64 +1210,64 @@
         <v>31</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0133940565260421</v>
+        <v>0.013</v>
       </c>
       <c r="C12" t="n">
-        <v>0.00561627874826428</v>
+        <v>0.006</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0158696631173649</v>
+        <v>0.016</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.00398650734168636</v>
+        <v>-0.004</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00777777777777778</v>
+        <v>0.008</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0521224853636869</v>
+        <v>0.052</v>
       </c>
       <c r="H12" t="n">
-        <v>0.147280133454403</v>
+        <v>0.147</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1077515530788</v>
+        <v>0.108</v>
       </c>
       <c r="J12" t="n">
-        <v>0.107785768727731</v>
+        <v>0.108</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0267052148823944</v>
+        <v>0.027</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0151259707845571</v>
+        <v>0.015</v>
       </c>
       <c r="M12" t="n">
-        <v>1.05476287922094</v>
+        <v>1.055</v>
       </c>
       <c r="N12" t="n">
-        <v>0.442133558239566</v>
+        <v>0.442</v>
       </c>
       <c r="O12" t="n">
-        <v>0.689104608006409</v>
+        <v>0.689</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.283371230088066</v>
+        <v>-0.283</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.122675735976218</v>
+        <v>-0.123</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0520005790186982</v>
+        <v>-0.052</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.119348487673923</v>
+        <v>-0.119</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.0860176441250002</v>
+        <v>-0.086</v>
       </c>
       <c r="U12" t="n">
-        <v>0.43562185659912</v>
+        <v>0.436</v>
       </c>
     </row>
     <row r="13">
@@ -1275,64 +1275,64 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0272709792138137</v>
+        <v>0.027</v>
       </c>
       <c r="C13" t="n">
-        <v>0.005104312547147</v>
+        <v>0.005</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0319663091769747</v>
+        <v>0.032</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.00449502514281778</v>
+        <v>-0.004</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0221666666666667</v>
+        <v>0.022</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0881951213299161</v>
+        <v>0.088</v>
       </c>
       <c r="H13" t="n">
-        <v>0.55233148250467</v>
+        <v>0.552</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0578752256380831</v>
+        <v>0.058</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0541097950609451</v>
+        <v>0.054</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0162541479294225</v>
+        <v>0.016</v>
       </c>
       <c r="L13" t="n">
-        <v>0.011945024730791</v>
+        <v>0.012</v>
       </c>
       <c r="M13" t="n">
-        <v>3.64992264532508</v>
+        <v>3.65</v>
       </c>
       <c r="N13" t="n">
-        <v>0.730696446610885</v>
+        <v>0.731</v>
       </c>
       <c r="O13" t="n">
-        <v>2.37852186187966</v>
+        <v>2.379</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.556950541003901</v>
+        <v>-0.557</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.147980233888225</v>
+        <v>0.148</v>
       </c>
       <c r="R13" t="n">
-        <v>0.0766785745084128</v>
+        <v>0.077</v>
       </c>
       <c r="S13" t="n">
-        <v>0.0861460072062545</v>
+        <v>0.086</v>
       </c>
       <c r="T13" t="n">
-        <v>0.145332170409591</v>
+        <v>0.145</v>
       </c>
       <c r="U13" t="n">
-        <v>0.723297774271687</v>
+        <v>0.723</v>
       </c>
     </row>
     <row r="14">
@@ -1340,64 +1340,64 @@
         <v>33</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0076961419396744</v>
+        <v>0.008</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.0588038580603256</v>
+        <v>-0.059</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.000786393834731465</v>
+        <v>-0.001</v>
       </c>
       <c r="E14" t="n">
-        <v>0.00873781225401459</v>
+        <v>0.009</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0665</v>
+        <v>0.066</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.13082007402315</v>
+        <v>-1.131</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.0151226460939026</v>
+        <v>-0.015</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0520010737438693</v>
+        <v>0.052</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0529831553914689</v>
+        <v>0.053</v>
       </c>
       <c r="K14" t="n">
-        <v>0.00856400033618865</v>
+        <v>0.009</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0306884287805184</v>
+        <v>0.031</v>
       </c>
       <c r="M14" t="n">
-        <v>1.14640054200502</v>
+        <v>1.146</v>
       </c>
       <c r="N14" t="n">
-        <v>-8.59693467773558</v>
+        <v>-8.597</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.102008077029556</v>
+        <v>-0.102</v>
       </c>
       <c r="P14" t="n">
-        <v>2.30190939572239</v>
+        <v>2.302</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.0915008386029681</v>
+        <v>0.092</v>
       </c>
       <c r="R14" t="n">
-        <v>0.139892486292301</v>
+        <v>0.14</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.0288152616354985</v>
+        <v>-0.029</v>
       </c>
       <c r="T14" t="n">
-        <v>0.0929893639529614</v>
+        <v>0.093</v>
       </c>
       <c r="U14" t="n">
-        <v>0.9101522410491</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="15">
@@ -1405,64 +1405,64 @@
         <v>34</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0147675304084191</v>
+        <v>0.015</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.107732469591581</v>
+        <v>-0.108</v>
       </c>
       <c r="D15" t="n">
-        <v>0.00487922145585897</v>
+        <v>0.005</v>
       </c>
       <c r="E15" t="n">
-        <v>0.00977223336363328</v>
+        <v>0.01</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1225</v>
+        <v>0.122</v>
       </c>
       <c r="G15" t="n">
-        <v>-3.30433609028986</v>
+        <v>-3.304</v>
       </c>
       <c r="H15" t="n">
-        <v>0.149653930799442</v>
+        <v>0.15</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0326033631712477</v>
+        <v>0.033</v>
       </c>
       <c r="J15" t="n">
-        <v>0.057531389615131</v>
+        <v>0.058</v>
       </c>
       <c r="K15" t="n">
-        <v>0.00985754769144441</v>
+        <v>0.01</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0367135037272691</v>
+        <v>0.037</v>
       </c>
       <c r="M15" t="n">
-        <v>3.50849690174646</v>
+        <v>3.508</v>
       </c>
       <c r="N15" t="n">
-        <v>-14.5049880896412</v>
+        <v>-14.505</v>
       </c>
       <c r="O15" t="n">
-        <v>0.572393455662776</v>
+        <v>0.572</v>
       </c>
       <c r="P15" t="n">
-        <v>2.07579658704648</v>
+        <v>2.076</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.0239820005593618</v>
+        <v>-0.024</v>
       </c>
       <c r="R15" t="n">
-        <v>0.520358572071996</v>
+        <v>0.52</v>
       </c>
       <c r="S15" t="n">
-        <v>-0.0459051319236111</v>
+        <v>-0.046</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.0962185770665585</v>
+        <v>-0.096</v>
       </c>
       <c r="U15" t="n">
-        <v>0.755632067997626</v>
+        <v>0.756</v>
       </c>
     </row>
     <row r="16">
@@ -1470,64 +1470,64 @@
         <v>35</v>
       </c>
       <c r="B16" t="n">
-        <v>0.009106332487633</v>
+        <v>0.009</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.2017270008457</v>
+        <v>-0.202</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.00399054348151866</v>
+        <v>-0.004</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0129442953101165</v>
+        <v>0.013</v>
       </c>
       <c r="F16" t="n">
-        <v>0.210833333333333</v>
+        <v>0.211</v>
       </c>
       <c r="G16" t="n">
-        <v>-5.94129429011561</v>
+        <v>-5.941</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.117530093154658</v>
+        <v>-0.118</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0339533763175658</v>
+        <v>0.034</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0875806005636399</v>
+        <v>0.088</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0110380868840142</v>
+        <v>0.011</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0710285611368775</v>
+        <v>0.071</v>
       </c>
       <c r="M16" t="n">
-        <v>2.07747669862121</v>
+        <v>2.077</v>
       </c>
       <c r="N16" t="n">
-        <v>-17.8415153522052</v>
+        <v>-17.842</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.500717081706216</v>
+        <v>-0.501</v>
       </c>
       <c r="P16" t="n">
-        <v>2.86564616474218</v>
+        <v>2.866</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.112842335979187</v>
+        <v>0.113</v>
       </c>
       <c r="R16" t="n">
-        <v>0.719596023129508</v>
+        <v>0.72</v>
       </c>
       <c r="S16" t="n">
-        <v>0.0105824307521963</v>
+        <v>0.011</v>
       </c>
       <c r="T16" t="n">
-        <v>0.0428756872563494</v>
+        <v>0.043</v>
       </c>
       <c r="U16" t="n">
-        <v>0.659915235771444</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="17">
@@ -1535,64 +1535,64 @@
         <v>36</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0132454913020873</v>
+        <v>0.013</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.239754508697913</v>
+        <v>-0.24</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0170548767276065</v>
+        <v>0.017</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.0030639482130764</v>
+        <v>-0.003</v>
       </c>
       <c r="F17" t="n">
         <v>0.253</v>
       </c>
       <c r="G17" t="n">
-        <v>-5.80686480178318</v>
+        <v>-5.807</v>
       </c>
       <c r="H17" t="n">
-        <v>0.413069868450617</v>
+        <v>0.413</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0412881162007231</v>
+        <v>0.041</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0684928096536633</v>
+        <v>0.068</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0108095950609627</v>
+        <v>0.011</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0551515631261185</v>
+        <v>0.055</v>
       </c>
       <c r="M17" t="n">
-        <v>2.48495557297529</v>
+        <v>2.485</v>
       </c>
       <c r="N17" t="n">
-        <v>-27.114239408793</v>
+        <v>-27.114</v>
       </c>
       <c r="O17" t="n">
-        <v>1.72496330928834</v>
+        <v>1.725</v>
       </c>
       <c r="P17" t="n">
-        <v>-0.554707819429069</v>
+        <v>-0.555</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.109000994293594</v>
+        <v>0.109</v>
       </c>
       <c r="R17" t="n">
-        <v>0.512260735927569</v>
+        <v>0.512</v>
       </c>
       <c r="S17" t="n">
-        <v>0.0304228473997883</v>
+        <v>0.03</v>
       </c>
       <c r="T17" t="n">
-        <v>0.0684533760873143</v>
+        <v>0.068</v>
       </c>
       <c r="U17" t="n">
-        <v>0.832414084888144</v>
+        <v>0.832</v>
       </c>
     </row>
     <row r="18">
@@ -1600,64 +1600,64 @@
         <v>37</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0089761394526426</v>
+        <v>0.009</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.434023860547357</v>
+        <v>-0.434</v>
       </c>
       <c r="D18" t="n">
-        <v>0.00714010201973936</v>
+        <v>0.007</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.000248008073443725</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
         <v>0.443</v>
       </c>
       <c r="G18" t="n">
-        <v>-7.27585975981063</v>
+        <v>-7.276</v>
       </c>
       <c r="H18" t="n">
-        <v>0.11969475802747</v>
+        <v>0.12</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0596525874433091</v>
+        <v>0.06</v>
       </c>
       <c r="J18" t="n">
-        <v>0.117347518492705</v>
+        <v>0.117</v>
       </c>
       <c r="K18" t="n">
-        <v>0.011544325303429</v>
+        <v>0.012</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0881889343148743</v>
+        <v>0.088</v>
       </c>
       <c r="M18" t="n">
-        <v>1.16556347690228</v>
+        <v>1.166</v>
       </c>
       <c r="N18" t="n">
-        <v>-28.6493861199299</v>
+        <v>-28.649</v>
       </c>
       <c r="O18" t="n">
-        <v>0.549769824995538</v>
+        <v>0.55</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.0340252382810983</v>
+        <v>-0.034</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.217994942955606</v>
+        <v>0.218</v>
       </c>
       <c r="R18" t="n">
-        <v>0.703357541612211</v>
+        <v>0.703</v>
       </c>
       <c r="S18" t="n">
-        <v>0.161063474121154</v>
+        <v>0.161</v>
       </c>
       <c r="T18" t="n">
-        <v>0.110495195956006</v>
+        <v>0.11</v>
       </c>
       <c r="U18" t="n">
-        <v>0.84409145744481</v>
+        <v>0.844</v>
       </c>
     </row>
     <row r="19">
@@ -1665,64 +1665,64 @@
         <v>38</v>
       </c>
       <c r="B19" t="n">
-        <v>0.00429975584527973</v>
+        <v>0.004</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.46520024415472</v>
+        <v>-0.465</v>
       </c>
       <c r="D19" t="n">
-        <v>0.00391870460952742</v>
+        <v>0.004</v>
       </c>
       <c r="E19" t="n">
-        <v>0.00192288532904467</v>
+        <v>0.002</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4695</v>
+        <v>0.47</v>
       </c>
       <c r="G19" t="n">
-        <v>-6.50987666185136</v>
+        <v>-6.51</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0548372104331215</v>
+        <v>0.055</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0714606847900588</v>
+        <v>0.071</v>
       </c>
       <c r="J19" t="n">
-        <v>0.170102508428989</v>
+        <v>0.17</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0132466732819786</v>
+        <v>0.013</v>
       </c>
       <c r="L19" t="n">
-        <v>0.142762395941352</v>
+        <v>0.143</v>
       </c>
       <c r="M19" t="n">
-        <v>0.466071178311547</v>
+        <v>0.466</v>
       </c>
       <c r="N19" t="n">
-        <v>-21.1838474917611</v>
+        <v>-21.184</v>
       </c>
       <c r="O19" t="n">
-        <v>0.240065043504028</v>
+        <v>0.24</v>
       </c>
       <c r="P19" t="n">
-        <v>0.220952276279784</v>
+        <v>0.221</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.114434669047225</v>
+        <v>0.114</v>
       </c>
       <c r="R19" t="n">
-        <v>0.703756545991021</v>
+        <v>0.704</v>
       </c>
       <c r="S19" t="n">
-        <v>-0.0706814743251702</v>
+        <v>-0.071</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.172848588262293</v>
+        <v>-0.173</v>
       </c>
       <c r="U19" t="n">
-        <v>0.829758703251184</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="20">
@@ -1730,64 +1730,64 @@
         <v>39</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0240623920159071</v>
+        <v>0.024</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.602437607984093</v>
+        <v>-0.602</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0323493423421379</v>
+        <v>0.032</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.00978471357426215</v>
+        <v>-0.01</v>
       </c>
       <c r="F20" t="n">
-        <v>0.6265</v>
+        <v>0.627</v>
       </c>
       <c r="G20" t="n">
-        <v>-10.3756984306794</v>
+        <v>-10.376</v>
       </c>
       <c r="H20" t="n">
-        <v>0.557148186176471</v>
+        <v>0.557</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0580623667899577</v>
+        <v>0.058</v>
       </c>
       <c r="J20" t="n">
-        <v>0.251918185864963</v>
+        <v>0.252</v>
       </c>
       <c r="K20" t="n">
-        <v>0.011119570305788</v>
+        <v>0.011</v>
       </c>
       <c r="L20" t="n">
-        <v>0.238802272651934</v>
+        <v>0.239</v>
       </c>
       <c r="M20" t="n">
-        <v>3.21010832660859</v>
+        <v>3.21</v>
       </c>
       <c r="N20" t="n">
-        <v>-18.5237188402279</v>
+        <v>-18.524</v>
       </c>
       <c r="O20" t="n">
-        <v>2.62499970078004</v>
+        <v>2.625</v>
       </c>
       <c r="P20" t="n">
-        <v>-1.55082785434244</v>
+        <v>-1.551</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.0441051545388317</v>
+        <v>0.044</v>
       </c>
       <c r="R20" t="n">
-        <v>0.842562422632455</v>
+        <v>0.843</v>
       </c>
       <c r="S20" t="n">
-        <v>0.114951548957138</v>
+        <v>0.115</v>
       </c>
       <c r="T20" t="n">
-        <v>0.269704232836712</v>
+        <v>0.27</v>
       </c>
       <c r="U20" t="n">
-        <v>0.897413818141607</v>
+        <v>0.897</v>
       </c>
     </row>
     <row r="21">
@@ -1795,64 +1795,64 @@
         <v>40</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0174235102121291</v>
+        <v>0.017</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.802743156454538</v>
+        <v>-0.803</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.00641720042603473</v>
+        <v>-0.006</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0228881602468667</v>
+        <v>0.023</v>
       </c>
       <c r="F21" t="n">
-        <v>0.820166666666667</v>
+        <v>0.82</v>
       </c>
       <c r="G21" t="n">
-        <v>-17.3406489345029</v>
+        <v>-17.341</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.138622694987139</v>
+        <v>-0.139</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0462925672209019</v>
+        <v>0.046</v>
       </c>
       <c r="J21" t="n">
-        <v>0.232800482613029</v>
+        <v>0.233</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0121320754264336</v>
+        <v>0.012</v>
       </c>
       <c r="L21" t="n">
-        <v>0.21639176389185</v>
+        <v>0.216</v>
       </c>
       <c r="M21" t="n">
-        <v>2.9154125137213</v>
+        <v>2.915</v>
       </c>
       <c r="N21" t="n">
-        <v>-26.7096600602699</v>
+        <v>-26.71</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.541495917643527</v>
+        <v>-0.541</v>
       </c>
       <c r="P21" t="n">
-        <v>3.41714848252989</v>
+        <v>3.417</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.219416132675625</v>
+        <v>0.219</v>
       </c>
       <c r="R21" t="n">
-        <v>0.88464372148355</v>
+        <v>0.885</v>
       </c>
       <c r="S21" t="n">
-        <v>0.0814360251570436</v>
+        <v>0.081</v>
       </c>
       <c r="T21" t="n">
-        <v>-0.0101951481759463</v>
+        <v>-0.01</v>
       </c>
       <c r="U21" t="n">
-        <v>0.895114600343766</v>
+        <v>0.895</v>
       </c>
     </row>
     <row r="22">
@@ -1860,64 +1860,64 @@
         <v>41</v>
       </c>
       <c r="B22" t="n">
-        <v>0.00785375265993704</v>
+        <v>0.008</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.544646247340063</v>
+        <v>-0.545</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.00530237978893098</v>
+        <v>-0.005</v>
       </c>
       <c r="E22" t="n">
-        <v>0.0128704612445035</v>
+        <v>0.013</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5525</v>
+        <v>0.552</v>
       </c>
       <c r="G22" t="n">
-        <v>-9.68807420537095</v>
+        <v>-9.688</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.0943178239290218</v>
+        <v>-0.094</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0562182159007533</v>
+        <v>0.056</v>
       </c>
       <c r="J22" t="n">
-        <v>0.131230553015532</v>
+        <v>0.131</v>
       </c>
       <c r="K22" t="n">
-        <v>0.011570524507304</v>
+        <v>0.012</v>
       </c>
       <c r="L22" t="n">
-        <v>0.107948905050931</v>
+        <v>0.108</v>
       </c>
       <c r="M22" t="n">
-        <v>1.08212090226651</v>
+        <v>1.082</v>
       </c>
       <c r="N22" t="n">
-        <v>-32.1480904720833</v>
+        <v>-32.148</v>
       </c>
       <c r="O22" t="n">
-        <v>-0.475134555133606</v>
+        <v>-0.475</v>
       </c>
       <c r="P22" t="n">
-        <v>2.53155850931159</v>
+        <v>2.532</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.210415719999514</v>
+        <v>0.21</v>
       </c>
       <c r="R22" t="n">
-        <v>0.606327593119062</v>
+        <v>0.606</v>
       </c>
       <c r="S22" t="n">
-        <v>0.211321179358934</v>
+        <v>0.211</v>
       </c>
       <c r="T22" t="n">
-        <v>0.14075957183144</v>
+        <v>0.141</v>
       </c>
       <c r="U22" t="n">
-        <v>0.791672039730449</v>
+        <v>0.792</v>
       </c>
     </row>
     <row r="23">
@@ -1925,64 +1925,64 @@
         <v>42</v>
       </c>
       <c r="B23" t="n">
-        <v>0.0173158246749331</v>
+        <v>0.017</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.333684175325067</v>
+        <v>-0.334</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0191137481515197</v>
+        <v>0.019</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.00157747521254153</v>
+        <v>-0.002</v>
       </c>
       <c r="F23" t="n">
         <v>0.351</v>
       </c>
       <c r="G23" t="n">
-        <v>-10.1919085054869</v>
+        <v>-10.192</v>
       </c>
       <c r="H23" t="n">
-        <v>0.583802250039078</v>
+        <v>0.584</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0327401070315167</v>
+        <v>0.033</v>
       </c>
       <c r="J23" t="n">
-        <v>0.0987214571710261</v>
+        <v>0.099</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0161562659828732</v>
+        <v>0.016</v>
       </c>
       <c r="L23" t="n">
-        <v>0.099177977325819</v>
+        <v>0.099</v>
       </c>
       <c r="M23" t="n">
-        <v>4.09674290479902</v>
+        <v>4.097</v>
       </c>
       <c r="N23" t="n">
-        <v>-26.1818107422797</v>
+        <v>-26.182</v>
       </c>
       <c r="O23" t="n">
-        <v>1.61044716438436</v>
+        <v>1.61</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.188002560019332</v>
+        <v>-0.188</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.233033765685642</v>
+        <v>0.233</v>
       </c>
       <c r="R23" t="n">
-        <v>0.814399918634215</v>
+        <v>0.814</v>
       </c>
       <c r="S23" t="n">
-        <v>0.332654313139402</v>
+        <v>0.333</v>
       </c>
       <c r="T23" t="n">
-        <v>0.323251205941965</v>
+        <v>0.323</v>
       </c>
       <c r="U23" t="n">
-        <v>0.905890237872636</v>
+        <v>0.906</v>
       </c>
     </row>
     <row r="24">
@@ -1990,64 +1990,64 @@
         <v>43</v>
       </c>
       <c r="B24" t="n">
-        <v>0.0109951754203298</v>
+        <v>0.011</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.410338157913004</v>
+        <v>-0.41</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00174239827525775</v>
+        <v>0.002</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0107199056040307</v>
+        <v>0.011</v>
       </c>
       <c r="F24" t="n">
-        <v>0.421333333333333</v>
+        <v>0.421</v>
       </c>
       <c r="G24" t="n">
-        <v>-10.0077223283147</v>
+        <v>-10.008</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0424952878201762</v>
+        <v>0.042</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0410021525829148</v>
+        <v>0.041</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0646956639626385</v>
+        <v>0.065</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0159219362373963</v>
+        <v>0.016</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0487979808788551</v>
+        <v>0.049</v>
       </c>
       <c r="M24" t="n">
-        <v>2.07716564175271</v>
+        <v>2.077</v>
       </c>
       <c r="N24" t="n">
-        <v>-49.1295012546209</v>
+        <v>-49.13</v>
       </c>
       <c r="O24" t="n">
-        <v>0.125356261757976</v>
+        <v>0.125</v>
       </c>
       <c r="P24" t="n">
-        <v>1.17037236525639</v>
+        <v>1.17</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.139989322599069</v>
+        <v>0.14</v>
       </c>
       <c r="R24" t="n">
-        <v>0.436383863312888</v>
+        <v>0.436</v>
       </c>
       <c r="S24" t="n">
-        <v>0.155907983490126</v>
+        <v>0.156</v>
       </c>
       <c r="T24" t="n">
-        <v>0.185203645486117</v>
+        <v>0.185</v>
       </c>
       <c r="U24" t="n">
-        <v>0.501190019326918</v>
+        <v>0.501</v>
       </c>
     </row>
     <row r="25">
@@ -2055,64 +2055,64 @@
         <v>44</v>
       </c>
       <c r="B25" t="n">
-        <v>0.0140711717621528</v>
+        <v>0.014</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.161262161571181</v>
+        <v>-0.161</v>
       </c>
       <c r="D25" t="n">
-        <v>0.00720638075545299</v>
+        <v>0.007</v>
       </c>
       <c r="E25" t="n">
-        <v>0.00674280876503357</v>
+        <v>0.007</v>
       </c>
       <c r="F25" t="n">
-        <v>0.175333333333333</v>
+        <v>0.175</v>
       </c>
       <c r="G25" t="n">
-        <v>-3.8022370921489</v>
+        <v>-3.802</v>
       </c>
       <c r="H25" t="n">
-        <v>0.169911949223358</v>
+        <v>0.17</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0424124423761382</v>
+        <v>0.042</v>
       </c>
       <c r="J25" t="n">
-        <v>0.115341114111751</v>
+        <v>0.115</v>
       </c>
       <c r="K25" t="n">
-        <v>0.00944663676383785</v>
+        <v>0.009</v>
       </c>
       <c r="L25" t="n">
-        <v>0.105307727703736</v>
+        <v>0.105</v>
       </c>
       <c r="M25" t="n">
-        <v>2.56987859426378</v>
+        <v>2.57</v>
       </c>
       <c r="N25" t="n">
-        <v>-10.8298878669312</v>
+        <v>-10.83</v>
       </c>
       <c r="O25" t="n">
-        <v>0.632226020430277</v>
+        <v>0.632</v>
       </c>
       <c r="P25" t="n">
-        <v>1.03961809102907</v>
+        <v>1.04</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.187778345704022</v>
+        <v>0.188</v>
       </c>
       <c r="R25" t="n">
-        <v>0.856087822233922</v>
+        <v>0.856</v>
       </c>
       <c r="S25" t="n">
-        <v>0.0158082858438587</v>
+        <v>0.016</v>
       </c>
       <c r="T25" t="n">
-        <v>-0.103637107142455</v>
+        <v>-0.104</v>
       </c>
       <c r="U25" t="n">
-        <v>0.953655477134076</v>
+        <v>0.954</v>
       </c>
     </row>
     <row r="26">
@@ -2120,64 +2120,64 @@
         <v>45</v>
       </c>
       <c r="B26" t="n">
-        <v>0.00919672805620422</v>
+        <v>0.009</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.174969938610462</v>
+        <v>-0.175</v>
       </c>
       <c r="D26" t="n">
-        <v>0.00382112764273743</v>
+        <v>0.004</v>
       </c>
       <c r="E26" t="n">
-        <v>0.00529595710341848</v>
+        <v>0.005</v>
       </c>
       <c r="F26" t="n">
-        <v>0.184166666666667</v>
+        <v>0.184</v>
       </c>
       <c r="G26" t="n">
-        <v>-2.63854652034684</v>
+        <v>-2.639</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0576226014915175</v>
+        <v>0.058</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0663130012153291</v>
+        <v>0.066</v>
       </c>
       <c r="J26" t="n">
-        <v>0.194251611521138</v>
+        <v>0.194</v>
       </c>
       <c r="K26" t="n">
-        <v>0.0131437500368849</v>
+        <v>0.013</v>
       </c>
       <c r="L26" t="n">
-        <v>0.177203241224773</v>
+        <v>0.177</v>
       </c>
       <c r="M26" t="n">
-        <v>1.07426217931586</v>
+        <v>1.074</v>
       </c>
       <c r="N26" t="n">
-        <v>-6.97709175248219</v>
+        <v>-6.977</v>
       </c>
       <c r="O26" t="n">
-        <v>0.243956055601774</v>
+        <v>0.244</v>
       </c>
       <c r="P26" t="n">
-        <v>0.685814152568716</v>
+        <v>0.686</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.321714548022094</v>
+        <v>0.322</v>
       </c>
       <c r="R26" t="n">
-        <v>0.904168607462086</v>
+        <v>0.904</v>
       </c>
       <c r="S26" t="n">
-        <v>0.329235649180592</v>
+        <v>0.329</v>
       </c>
       <c r="T26" t="n">
-        <v>0.259586432593983</v>
+        <v>0.26</v>
       </c>
       <c r="U26" t="n">
-        <v>0.985564368147097</v>
+        <v>0.986</v>
       </c>
     </row>
     <row r="27">
@@ -2185,64 +2185,64 @@
         <v>46</v>
       </c>
       <c r="B27" t="n">
-        <v>0.00600527312899951</v>
+        <v>0.006</v>
       </c>
       <c r="C27" t="n">
-        <v>0.00417193979566617</v>
+        <v>0.004</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.0062318315464091</v>
+        <v>-0.006</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0134026710506118</v>
+        <v>0.013</v>
       </c>
       <c r="F27" t="n">
-        <v>0.00183333333333333</v>
+        <v>0.002</v>
       </c>
       <c r="G27" t="n">
-        <v>0.10721358719405</v>
+        <v>0.107</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.160150205325021</v>
+        <v>-0.16</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0389124168386907</v>
+        <v>0.039</v>
       </c>
       <c r="J27" t="n">
-        <v>0.0394839427621954</v>
+        <v>0.039</v>
       </c>
       <c r="K27" t="n">
-        <v>0.00735807218289583</v>
+        <v>0.007</v>
       </c>
       <c r="L27" t="n">
-        <v>0.00390204929499423</v>
+        <v>0.004</v>
       </c>
       <c r="M27" t="n">
-        <v>1.19541908252361</v>
+        <v>1.195</v>
       </c>
       <c r="N27" t="n">
-        <v>0.818451867753476</v>
+        <v>0.818</v>
       </c>
       <c r="O27" t="n">
-        <v>-0.713728438406984</v>
+        <v>-0.714</v>
       </c>
       <c r="P27" t="n">
-        <v>2.89551309131106</v>
+        <v>2.896</v>
       </c>
       <c r="Q27" t="n">
-        <v>-0.101453761929764</v>
+        <v>-0.101</v>
       </c>
       <c r="R27" t="n">
-        <v>-0.104902308705517</v>
+        <v>-0.105</v>
       </c>
       <c r="S27" t="n">
-        <v>-0.0664688954910906</v>
+        <v>-0.066</v>
       </c>
       <c r="T27" t="n">
-        <v>-0.0813696483829692</v>
+        <v>-0.081</v>
       </c>
       <c r="U27" t="n">
-        <v>0.518367346938775</v>
+        <v>0.518</v>
       </c>
     </row>
     <row r="28">
@@ -2250,64 +2250,64 @@
         <v>47</v>
       </c>
       <c r="B28" t="n">
-        <v>0.010788071548205</v>
+        <v>0.011</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.0790452617851284</v>
+        <v>-0.079</v>
       </c>
       <c r="D28" t="n">
-        <v>0.00348268456349802</v>
+        <v>0.003</v>
       </c>
       <c r="E28" t="n">
-        <v>0.00693980384850374</v>
+        <v>0.007</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0898333333333333</v>
+        <v>0.09</v>
       </c>
       <c r="G28" t="n">
-        <v>-1.2931281560307</v>
+        <v>-1.293</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0569744139740465</v>
+        <v>0.057</v>
       </c>
       <c r="I28" t="n">
-        <v>0.0611271678035071</v>
+        <v>0.061</v>
       </c>
       <c r="J28" t="n">
-        <v>0.105838764591702</v>
+        <v>0.106</v>
       </c>
       <c r="K28" t="n">
-        <v>0.00817579658875559</v>
+        <v>0.008</v>
       </c>
       <c r="L28" t="n">
-        <v>0.0704583460710897</v>
+        <v>0.07</v>
       </c>
       <c r="M28" t="n">
-        <v>1.36705242350504</v>
+        <v>1.367</v>
       </c>
       <c r="N28" t="n">
-        <v>-5.78504451882858</v>
+        <v>-5.785</v>
       </c>
       <c r="O28" t="n">
-        <v>0.287975879438566</v>
+        <v>0.288</v>
       </c>
       <c r="P28" t="n">
-        <v>1.28143282794518</v>
+        <v>1.281</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.0366313561860626</v>
+        <v>-0.037</v>
       </c>
       <c r="R28" t="n">
-        <v>0.547626919856167</v>
+        <v>0.548</v>
       </c>
       <c r="S28" t="n">
-        <v>-0.125612012880184</v>
+        <v>-0.126</v>
       </c>
       <c r="T28" t="n">
-        <v>-0.164132860512695</v>
+        <v>-0.164</v>
       </c>
       <c r="U28" t="n">
-        <v>0.947279656302888</v>
+        <v>0.947</v>
       </c>
     </row>
     <row r="29">
@@ -2315,64 +2315,64 @@
         <v>48</v>
       </c>
       <c r="B29" t="n">
-        <v>0.00269764289839517</v>
+        <v>0.003</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.0573023571016048</v>
+        <v>-0.057</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0122153779840781</v>
+        <v>0.012</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.00320784147981004</v>
+        <v>-0.003</v>
       </c>
       <c r="F29" t="n">
         <v>0.06</v>
       </c>
       <c r="G29" t="n">
-        <v>-1.14083128575792</v>
+        <v>-1.141</v>
       </c>
       <c r="H29" t="n">
-        <v>0.243195674252717</v>
+        <v>0.243</v>
       </c>
       <c r="I29" t="n">
-        <v>0.0502285989321687</v>
+        <v>0.05</v>
       </c>
       <c r="J29" t="n">
-        <v>0.117938334631123</v>
+        <v>0.118</v>
       </c>
       <c r="K29" t="n">
-        <v>0.00633353397574908</v>
+        <v>0.006</v>
       </c>
       <c r="L29" t="n">
-        <v>0.102787243329629</v>
+        <v>0.103</v>
       </c>
       <c r="M29" t="n">
-        <v>0.263111006470016</v>
+        <v>0.263</v>
       </c>
       <c r="N29" t="n">
-        <v>-2.38025297536532</v>
+        <v>-2.38</v>
       </c>
       <c r="O29" t="n">
-        <v>1.15238896053049</v>
+        <v>1.152</v>
       </c>
       <c r="P29" t="n">
-        <v>-0.386305425443892</v>
+        <v>-0.386</v>
       </c>
       <c r="Q29" t="n">
-        <v>-0.218055610184782</v>
+        <v>-0.218</v>
       </c>
       <c r="R29" t="n">
-        <v>0.705057212970736</v>
+        <v>0.705</v>
       </c>
       <c r="S29" t="n">
-        <v>0.0330010361262094</v>
+        <v>0.033</v>
       </c>
       <c r="T29" t="n">
-        <v>-0.0200879184112616</v>
+        <v>-0.02</v>
       </c>
       <c r="U29" t="n">
-        <v>0.975367833259343</v>
+        <v>0.975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>